<commit_message>
feat: add viewCount and likeCount fields
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,16 @@
           <t>videoId</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>viewCount</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>likeCount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -476,6 +486,16 @@
           <t>hHOitwOK28g</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>209043</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>18691</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -498,6 +518,16 @@
           <t>X_PhdTyRwBQ</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>50375</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>3597</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -520,6 +550,16 @@
           <t>T_5bSm9ft8o</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>15949</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>1143</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -542,6 +582,16 @@
           <t>AO5mD8zTNQM</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>6307</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>615</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -564,6 +614,16 @@
           <t>omeGkWLmkHk</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>199233</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>12673</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -586,6 +646,16 @@
           <t>AbVDlYyQjs8</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>11190</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>792</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -608,6 +678,16 @@
           <t>szqrds4VXRw</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>115609</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>8145</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -630,6 +710,16 @@
           <t>2x1QpHaj7M0</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>526715</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>55379</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -652,6 +742,16 @@
           <t>1k3jEKbu04o</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -674,6 +774,16 @@
           <t>tuogEwQQm-4</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>9705</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>402</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -696,6 +806,16 @@
           <t>8xpuMV2VPcA</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1140324</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>42325</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -718,26 +838,46 @@
           <t>3YizcFDuMV8</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>164999</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>9168</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Como a reforma agrária ajudou a moldar a principal economia capitalista do mundo</t>
+          <t>REFORMA AGRÁRIA | Ciro Responde #1</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Você sabia que nos Estados Unidos foi feita reforma agrária? Ela aconteceu mais de 160 anos atrás e ajudou a moldar a ...</t>
+          <t>A reforma agrária no Brasil precisa ser feita em novos moldes. Além da terra, o pequeno produtor precisa ter acesso a crédito, ...</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Brasil de Fato</t>
+          <t>Ciro Gomes</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ExMxlNTp3mc</t>
+          <t>zRuywIMlEG4</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>13450</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>1199</t>
         </is>
       </c>
     </row>
@@ -762,26 +902,46 @@
           <t>oLYG_wdzhkQ</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>15718</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>596</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>REFORMA AGRÁRIA | Ciro Responde #1</t>
+          <t>Como a reforma agrária ajudou a moldar a principal economia capitalista do mundo</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>A reforma agrária no Brasil precisa ser feita em novos moldes. Além da terra, o pequeno produtor precisa ter acesso a crédito, ...</t>
+          <t>Você sabia que nos Estados Unidos foi feita reforma agrária? Ela aconteceu mais de 160 anos atrás e ajudou a moldar a ...</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Ciro Gomes</t>
+          <t>Brasil de Fato</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>zRuywIMlEG4</t>
+          <t>ExMxlNTp3mc</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>9841</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>696</t>
         </is>
       </c>
     </row>
@@ -806,6 +966,16 @@
           <t>HApn-pXavKM</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>23237</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2680</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -828,6 +998,16 @@
           <t>5kM02Bs1rds</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>48754</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>1579</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -850,6 +1030,16 @@
           <t>ZLE-3GbYqEg</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>11674</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>304</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -872,6 +1062,16 @@
           <t>HzvAq5Hd6lg</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>7009</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>252</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -894,6 +1094,16 @@
           <t>6ZOmreL1Y8o</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>44049</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>11402</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -916,6 +1126,16 @@
           <t>GbSJJGT2Vmc</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>23930</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>796</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -938,92 +1158,142 @@
           <t>s7ltqE5nnjA</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>6120</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Por que é tão difícil implementar a reforma agrária? | Meio Explica</t>
+          <t>Entenda a Reforma Agrária no Brasil: História, Desafios e Impactos</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>É estrutural a desigualdade na distribuição de terras em nosso país. No âmbito das políticas públicas, no entanto, pouco tem sido ...</t>
+          <t>Neste vídeo, você vai entender o que é a Reforma Agrária no Brasil, sua importância para a distribuição de terras, os desafios ...</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Meio</t>
+          <t>Outro lado da História</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Zvbmiar6XsQ</t>
+          <t>O2zsRwSGFbM</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>8512</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>399</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Entenda a Reforma Agrária no Brasil: História, Desafios e Impactos</t>
+          <t>Por que é tão difícil implementar a reforma agrária? | Meio Explica</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Neste vídeo, você vai entender o que é a Reforma Agrária no Brasil, sua importância para a distribuição de terras, os desafios ...</t>
+          <t>É estrutural a desigualdade na distribuição de terras em nosso país. No âmbito das políticas públicas, no entanto, pouco tem sido ...</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Outro lado da História</t>
+          <t>Meio</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>O2zsRwSGFbM</t>
+          <t>Zvbmiar6XsQ</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>5076</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>558</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>&amp;quot;A feira da Reforma Agrária é um marco na luta contra a CPI do MST&amp;quot;, João Paulo Rodrigues</t>
+          <t>&amp;quot;Governo Bolsonaro é contra a reforma agrária e defende grileiros&amp;quot;</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Para João Paulo Rodrigues, a Feira do MST é como uma "prestação de conta" à sociedade, uma vez que as famílias ...</t>
+          <t>A convidada do Entre Vistas desta semana foi a coordenadora de políticas públicas do Greenpeace Brasil, Mariana Mota. Confira ...</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Brasil de Fato</t>
+          <t>Rede TVT</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>u9QjU3rDMyw</t>
+          <t>DVVAQ3jj6Xk</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>4532</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>498</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>&amp;quot;Governo Bolsonaro é contra a reforma agrária e defende grileiros&amp;quot;</t>
+          <t>&amp;quot;A feira da Reforma Agrária é um marco na luta contra a CPI do MST&amp;quot;, João Paulo Rodrigues</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>A convidada do Entre Vistas desta semana foi a coordenadora de políticas públicas do Greenpeace Brasil, Mariana Mota. Confira ...</t>
+          <t>Para João Paulo Rodrigues, a Feira do MST é como uma "prestação de conta" à sociedade, uma vez que as famílias ...</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Rede TVT</t>
+          <t>Brasil de Fato</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>DVVAQ3jj6Xk</t>
+          <t>u9QjU3rDMyw</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>1321</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>103</t>
         </is>
       </c>
     </row>
@@ -1048,6 +1318,16 @@
           <t>lBHwIaUWQhE</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>7521</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>447</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1070,6 +1350,16 @@
           <t>5gN4tEo-baU</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>7079</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>428</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1092,84 +1382,134 @@
           <t>RkD2CdjG9sY</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>242</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Cra Tabôa | Ela era contra a reforma agrária</t>
+          <t>Reforma Agrária - Sala Debate - Canal Futura - Parte 01</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Conheça a história de Nágila, uma das produtoras que faz parte do CRA Tabôa. -- O que é o CRA Tabôa? -- Investimento de ...</t>
+          <t>REFORMA ÁGRARIA O debate sobre a reforma agrária se confunde com a história republicana brasileira, principalmente depois ...</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Grupo Gaia</t>
+          <t>Canal Futura</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>ZvXuKeZD06M</t>
+          <t>LoCB3RSoNIw</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>19061</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>344</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>REFORMA AGRÁRIA | Lula solicita levantamento de terras que possam ser direcionadas a trabalhadores</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr"/>
+          <t>Cra Tabôa | Ela era contra a reforma agrária</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Conheça a história de Nágila, uma das produtoras que faz parte do CRA Tabôa. -- O que é o CRA Tabôa? -- Investimento de ...</t>
+        </is>
+      </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CanalGov</t>
+          <t>Grupo Gaia</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>VfusRR4rkE8</t>
+          <t>ZvXuKeZD06M</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>1062</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>63</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Reforma Agrária - Sala Debate - Canal Futura - Parte 01</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>REFORMA ÁGRARIA O debate sobre a reforma agrária se confunde com a história republicana brasileira, principalmente depois ...</t>
-        </is>
-      </c>
+          <t>Socialismo e Reforma Agrária</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Canal Futura</t>
+          <t>Humberto Matos</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>LoCB3RSoNIw</t>
+          <t>ILinUnuQFRE</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>5030</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>809</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Socialismo e Reforma Agrária</t>
+          <t>REFORMA AGRÁRIA | Lula solicita levantamento de terras que possam ser direcionadas a trabalhadores</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Humberto Matos</t>
+          <t>CanalGov</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>ILinUnuQFRE</t>
+          <t>VfusRR4rkE8</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>15771</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -1190,6 +1530,16 @@
           <t>935zD_PV6-o</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>5356</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1212,6 +1562,16 @@
           <t>R0HFo5cpwUs</t>
         </is>
       </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>15325</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>1584</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1234,48 +1594,78 @@
           <t>YX0gjNlPTUI</t>
         </is>
       </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>44903</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>1735</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>#AprueboWallmapu Breve historia de la contra reforma agraria. Joana Salém, Brasil.</t>
+          <t>O MST e a reforma agrária popular: a luta contra a criminalização</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>wallmapusinforestales #wallmapu #plurinacionalidad #Plurinacional #AprueboDeSalida ...</t>
+          <t>As ocupações de terra, as mobilizações, a luta por educação, a produção de alimentos saudáveis e outras ações marcam a ...</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Revista De Frente</t>
+          <t>TV 247</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>awfVX6JRDfI</t>
+          <t>ZVn9kCUMigA</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>726</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>125</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>O MST e a reforma agrária popular: a luta contra a criminalização</t>
+          <t>#AprueboWallmapu Breve historia de la contra reforma agraria. Joana Salém, Brasil.</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>As ocupações de terra, as mobilizações, a luta por educação, a produção de alimentos saudáveis e outras ações marcam a ...</t>
+          <t>wallmapusinforestales #wallmapu #plurinacionalidad #Plurinacional #AprueboDeSalida ...</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TV 247</t>
+          <t>Revista De Frente</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>ZVn9kCUMigA</t>
+          <t>awfVX6JRDfI</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>2</t>
         </is>
       </c>
     </row>
@@ -1300,6 +1690,16 @@
           <t>nReHoi4JofA</t>
         </is>
       </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>185128</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>3802</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1320,6 +1720,16 @@
       <c r="D41" t="inlineStr">
         <is>
           <t>8je9YJrMOmo</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>410</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>